<commit_message>
shorter names on output data and fixed matlab list data
</commit_message>
<xml_diff>
--- a/ass2/warm-up-table.xlsx
+++ b/ass2/warm-up-table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>blocked</t>
   </si>
@@ -36,6 +36,12 @@
     <t>t=10 000</t>
   </si>
   <si>
+    <t>0.50916</t>
+  </si>
+  <si>
+    <t>1.3548</t>
+  </si>
+  <si>
     <t>t= 4000</t>
   </si>
   <si>
@@ -61,13 +67,70 @@
   </si>
   <si>
     <t>11 ch 0 res</t>
+  </si>
+  <si>
+    <t>b%</t>
+  </si>
+  <si>
+    <t>d%</t>
+  </si>
+  <si>
+    <t>1.6211</t>
+  </si>
+  <si>
+    <t>0.80652</t>
+  </si>
+  <si>
+    <t>3.8111</t>
+  </si>
+  <si>
+    <t>0.35490</t>
+  </si>
+  <si>
+    <t>0.20325</t>
+  </si>
+  <si>
+    <t>0.57261</t>
+  </si>
+  <si>
+    <t>11 ch 1 res</t>
+  </si>
+  <si>
+    <t>0.69623</t>
+  </si>
+  <si>
+    <t>0.35842</t>
+  </si>
+  <si>
+    <t>11 ch 2 res</t>
+  </si>
+  <si>
+    <t>1.7704</t>
+  </si>
+  <si>
+    <t>0.16937</t>
+  </si>
+  <si>
+    <t>limit 2%</t>
+  </si>
+  <si>
+    <t>limit 1%</t>
+  </si>
+  <si>
+    <t>11 ch 3 res</t>
+  </si>
+  <si>
+    <t>3.9027</t>
+  </si>
+  <si>
+    <t>0.059419</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,13 +168,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,11 +218,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -474,17 +564,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -515,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -765,7 +855,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E17">
         <v>600</v>
@@ -991,33 +1081,106 @@
         <v>1.1782999999999999</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F29">
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
+    <row r="32" spans="1:8">
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="C34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="C36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="C37" t="s">
+      <c r="C35" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="C37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="C38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="C39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="C40" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>